<commit_message>
Update user story points
</commit_message>
<xml_diff>
--- a/User story points.xlsx
+++ b/User story points.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris Yang\Documents\GitHub\IFB299-42\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="4" activeTab="5"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Total" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Release1" sheetId="2" r:id="rId4"/>
-    <sheet state="visible" name="Database 1-2" sheetId="3" r:id="rId5"/>
-    <sheet state="visible" name="Release 2" sheetId="4" r:id="rId6"/>
-    <sheet state="visible" name="Release 3" sheetId="5" r:id="rId7"/>
-    <sheet state="visible" name="Release 4" sheetId="6" r:id="rId8"/>
+    <sheet name="Total" sheetId="1" r:id="rId1"/>
+    <sheet name="Release1" sheetId="2" r:id="rId2"/>
+    <sheet name="Database 1-2" sheetId="3" r:id="rId3"/>
+    <sheet name="Release 2" sheetId="4" r:id="rId4"/>
+    <sheet name="Release 3" sheetId="5" r:id="rId5"/>
+    <sheet name="Release 4" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Total!$A$1:$D$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Total!$A$1:$D$45</definedName>
   </definedNames>
-  <calcPr/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="83">
   <si>
     <t>Redemption for storage expansion</t>
   </si>
@@ -258,40 +267,80 @@
   </si>
   <si>
     <t>Personal media vault display DIY</t>
+  </si>
+  <si>
+    <t>This is not a user story</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>This is not a user story</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>This is not user story</t>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
-    </font>
-    <font/>
-    <font>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color rgb="FFFF0000"/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
-      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF434343"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -299,7 +348,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -320,6 +369,7 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -334,6 +384,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -344,6 +395,7 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -352,107 +404,410 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+  <cellXfs count="22">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/worksheetdrawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/worksheetdrawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/worksheetdrawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/worksheetdrawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/worksheetdrawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="CCE8CF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A2:Z51"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="43.86"/>
+    <col min="2" max="2" width="43.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -461,12 +816,12 @@
         <v>1</v>
       </c>
       <c r="D2" s="1">
-        <v>16.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -475,14 +830,14 @@
         <v>1</v>
       </c>
       <c r="D3" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
@@ -491,12 +846,12 @@
         <v>1</v>
       </c>
       <c r="D4" s="1">
-        <v>16.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
@@ -505,13 +860,13 @@
         <v>1</v>
       </c>
       <c r="D5" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>34.0</v>
+        <v>34</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
@@ -520,13 +875,13 @@
         <v>1</v>
       </c>
       <c r="D6" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
@@ -535,13 +890,13 @@
         <v>1</v>
       </c>
       <c r="D7" s="3">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
@@ -550,13 +905,13 @@
         <v>1</v>
       </c>
       <c r="D8" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="H8" s="2"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>41.0</v>
+        <v>41</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>8</v>
@@ -565,13 +920,13 @@
         <v>1</v>
       </c>
       <c r="D9" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="H9" s="2"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
@@ -580,12 +935,12 @@
         <v>10</v>
       </c>
       <c r="D10" s="1">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>11</v>
@@ -594,12 +949,12 @@
         <v>10</v>
       </c>
       <c r="D11" s="1">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>12</v>
@@ -608,12 +963,12 @@
         <v>10</v>
       </c>
       <c r="D12" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>13</v>
@@ -622,12 +977,12 @@
         <v>10</v>
       </c>
       <c r="D13" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>14</v>
@@ -636,12 +991,12 @@
         <v>10</v>
       </c>
       <c r="D14" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>15</v>
@@ -650,12 +1005,12 @@
         <v>10</v>
       </c>
       <c r="D15" s="1">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>16</v>
@@ -664,7 +1019,7 @@
         <v>10</v>
       </c>
       <c r="D16" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -689,9 +1044,9 @@
       <c r="Y16" s="5"/>
       <c r="Z16" s="5"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>17</v>
@@ -700,12 +1055,12 @@
         <v>10</v>
       </c>
       <c r="D17" s="1">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>18</v>
@@ -714,12 +1069,12 @@
         <v>10</v>
       </c>
       <c r="D18" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>19</v>
@@ -728,12 +1083,12 @@
         <v>10</v>
       </c>
       <c r="D19" s="1">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>20</v>
@@ -742,12 +1097,12 @@
         <v>10</v>
       </c>
       <c r="D20" s="1">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>21</v>
@@ -756,13 +1111,13 @@
         <v>10</v>
       </c>
       <c r="D21" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K21" s="2"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>22</v>
@@ -771,12 +1126,12 @@
         <v>10</v>
       </c>
       <c r="D22" s="1">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>23</v>
@@ -785,12 +1140,12 @@
         <v>10</v>
       </c>
       <c r="D23" s="1">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>24</v>
@@ -799,12 +1154,12 @@
         <v>10</v>
       </c>
       <c r="D24" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>25</v>
@@ -813,12 +1168,12 @@
         <v>10</v>
       </c>
       <c r="D25" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>26</v>
@@ -827,12 +1182,12 @@
         <v>10</v>
       </c>
       <c r="D26" s="1">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>27</v>
@@ -841,12 +1196,12 @@
         <v>10</v>
       </c>
       <c r="D27" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>28</v>
@@ -855,12 +1210,12 @@
         <v>10</v>
       </c>
       <c r="D28" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>29</v>
@@ -869,12 +1224,12 @@
         <v>10</v>
       </c>
       <c r="D29" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>30</v>
@@ -883,12 +1238,12 @@
         <v>10</v>
       </c>
       <c r="D30" s="1">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="31">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>31</v>
@@ -897,12 +1252,12 @@
         <v>32</v>
       </c>
       <c r="D31" s="1">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>33</v>
@@ -911,12 +1266,12 @@
         <v>32</v>
       </c>
       <c r="D32" s="1">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>34</v>
@@ -925,12 +1280,12 @@
         <v>32</v>
       </c>
       <c r="D33" s="1">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="34">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>35</v>
@@ -939,12 +1294,12 @@
         <v>32</v>
       </c>
       <c r="D34" s="1">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>36</v>
@@ -953,12 +1308,12 @@
         <v>32</v>
       </c>
       <c r="D35" s="1">
-        <v>16.0</v>
-      </c>
-    </row>
-    <row r="36">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>37</v>
@@ -967,12 +1322,12 @@
         <v>32</v>
       </c>
       <c r="D36" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>38</v>
@@ -981,12 +1336,12 @@
         <v>32</v>
       </c>
       <c r="D37" s="1">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="38">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>39</v>
@@ -995,12 +1350,12 @@
         <v>32</v>
       </c>
       <c r="D38" s="1">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="39">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>40</v>
@@ -1009,12 +1364,12 @@
         <v>32</v>
       </c>
       <c r="D39" s="1">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>41</v>
@@ -1023,12 +1378,12 @@
         <v>32</v>
       </c>
       <c r="D40" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>44</v>
@@ -1037,12 +1392,12 @@
         <v>32</v>
       </c>
       <c r="D41" s="1">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>46</v>
@@ -1051,12 +1406,12 @@
         <v>32</v>
       </c>
       <c r="D42" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>47</v>
@@ -1065,18 +1420,18 @@
         <v>32</v>
       </c>
       <c r="D43" s="1">
-        <v>16.0</v>
-      </c>
-    </row>
-    <row r="44" hidden="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="14.25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="6"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
     </row>
-    <row r="45">
+    <row r="45" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>49</v>
@@ -1085,10 +1440,10 @@
         <v>32</v>
       </c>
       <c r="D45" s="1">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F46" s="2" t="s">
         <v>50</v>
       </c>
@@ -1099,87 +1454,92 @@
         <v>52</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F47" s="2">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="G47" s="2">
-        <v>255.0</v>
-      </c>
-      <c r="I47" t="str">
+        <v>255</v>
+      </c>
+      <c r="I47">
         <f>255/4</f>
         <v>63.75</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="E48" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F48" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="G48" s="2">
-        <v>82.0</v>
-      </c>
-    </row>
-    <row r="49">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="5:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="E49" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F49" s="2">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="G49" s="2">
-        <v>87.0</v>
-      </c>
-    </row>
-    <row r="50">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50" spans="5:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="E50" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F50" s="2">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="G50" s="2">
-        <v>86.0</v>
-      </c>
-    </row>
-    <row r="51">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="51" spans="5:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="E51" s="2" t="s">
         <v>53</v>
       </c>
       <c r="F51" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G51" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$D$45">
+  <autoFilter ref="A1:D45">
     <filterColumn colId="2">
       <filters>
-        <filter val="Should"/>
         <filter val="Could"/>
         <filter val="Must"/>
+        <filter val="Should"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <drawing r:id="rId1"/>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:D24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="44.71"/>
+    <col min="2" max="2" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>42</v>
       </c>
@@ -1190,17 +1550,17 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>48</v>
       </c>
@@ -1209,9 +1569,9 @@
       <c r="D4" s="10"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>12</v>
@@ -1220,16 +1580,16 @@
         <v>10</v>
       </c>
       <c r="D5" s="6">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>54</v>
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>30</v>
@@ -1238,15 +1598,15 @@
         <v>10</v>
       </c>
       <c r="D6" s="6">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>13</v>
@@ -1255,13 +1615,13 @@
         <v>10</v>
       </c>
       <c r="D7" s="6">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>14</v>
@@ -1270,16 +1630,16 @@
         <v>10</v>
       </c>
       <c r="D8" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>57</v>
       </c>
       <c r="H8" s="2"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>15</v>
@@ -1288,17 +1648,17 @@
         <v>10</v>
       </c>
       <c r="D9" s="6">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="H9" s="2"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>59</v>
       </c>
@@ -1306,9 +1666,9 @@
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>21</v>
@@ -1317,15 +1677,15 @@
         <v>10</v>
       </c>
       <c r="D13" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="12" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>17</v>
@@ -1334,15 +1694,15 @@
         <v>10</v>
       </c>
       <c r="D14" s="6">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E14" s="12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>18</v>
@@ -1351,15 +1711,15 @@
         <v>10</v>
       </c>
       <c r="D15" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>19</v>
@@ -1368,12 +1728,12 @@
         <v>10</v>
       </c>
       <c r="D16" s="6">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>20</v>
@@ -1382,24 +1742,24 @@
         <v>10</v>
       </c>
       <c r="D17" s="6">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>22</v>
@@ -1408,15 +1768,15 @@
         <v>10</v>
       </c>
       <c r="D21" s="6">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>23</v>
@@ -1425,16 +1785,16 @@
         <v>10</v>
       </c>
       <c r="D22" s="6">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E22" s="12" t="s">
         <v>63</v>
       </c>
       <c r="H22" s="2"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>27</v>
@@ -1443,13 +1803,13 @@
         <v>10</v>
       </c>
       <c r="D23" s="6">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>28</v>
@@ -1458,35 +1818,38 @@
         <v>10</v>
       </c>
       <c r="D24" s="6">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E24" s="2"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="B28" s="6" t="s">
+    <row r="28" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A28" s="18">
+        <v>1</v>
+      </c>
+      <c r="B28" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="6">
-        <v>8.0</v>
-      </c>
-      <c r="E28" s="12" t="s">
+      <c r="C28" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="18">
+        <v>8</v>
+      </c>
+      <c r="E28" s="19" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="29">
+      <c r="F28" s="18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>24</v>
@@ -1495,12 +1858,12 @@
         <v>10</v>
       </c>
       <c r="D29" s="6">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>29</v>
@@ -1509,46 +1872,48 @@
         <v>10</v>
       </c>
       <c r="D30" s="6">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C32" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D32" s="2">
-        <v>67.0</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="46.0"/>
+    <col min="2" max="2" width="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>24</v>
@@ -1557,7 +1922,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="7">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
@@ -1582,9 +1947,9 @@
       <c r="Y3" s="11"/>
       <c r="Z3" s="11"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>29</v>
@@ -1593,7 +1958,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="7">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>55</v>
@@ -1620,7 +1985,7 @@
       <c r="Y5" s="11"/>
       <c r="Z5" s="11"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -1648,7 +2013,7 @@
       <c r="Y6" s="11"/>
       <c r="Z6" s="11"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1676,9 +2041,9 @@
       <c r="Y7" s="11"/>
       <c r="Z7" s="11"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>21</v>
@@ -1687,7 +2052,7 @@
         <v>10</v>
       </c>
       <c r="D8" s="7">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>58</v>
@@ -1714,9 +2079,9 @@
       <c r="Y8" s="11"/>
       <c r="Z8" s="11"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>22</v>
@@ -1725,7 +2090,7 @@
         <v>10</v>
       </c>
       <c r="D9" s="7">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>60</v>
@@ -1752,9 +2117,9 @@
       <c r="Y9" s="11"/>
       <c r="Z9" s="11"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>23</v>
@@ -1763,7 +2128,7 @@
         <v>10</v>
       </c>
       <c r="D10" s="7">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>63</v>
@@ -1790,9 +2155,9 @@
       <c r="Y10" s="11"/>
       <c r="Z10" s="11"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>27</v>
@@ -1801,7 +2166,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="7">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="11"/>
@@ -1826,9 +2191,9 @@
       <c r="Y11" s="11"/>
       <c r="Z11" s="11"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>28</v>
@@ -1837,7 +2202,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="7">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="11"/>
@@ -1862,9 +2227,9 @@
       <c r="Y12" s="11"/>
       <c r="Z12" s="11"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>17</v>
@@ -1873,7 +2238,7 @@
         <v>10</v>
       </c>
       <c r="D13" s="7">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>61</v>
@@ -1900,9 +2265,9 @@
       <c r="Y13" s="11"/>
       <c r="Z13" s="11"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>18</v>
@@ -1911,7 +2276,7 @@
         <v>10</v>
       </c>
       <c r="D14" s="7">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="13" t="s">
         <v>62</v>
@@ -1938,14 +2303,14 @@
       <c r="Y14" s="11"/>
       <c r="Z14" s="11"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>46</v>
@@ -1954,7 +2319,7 @@
         <v>32</v>
       </c>
       <c r="D17" s="7">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
@@ -1979,9 +2344,9 @@
       <c r="Y17" s="11"/>
       <c r="Z17" s="11"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>16</v>
@@ -1990,7 +2355,7 @@
         <v>10</v>
       </c>
       <c r="D18" s="7">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
@@ -2015,9 +2380,9 @@
       <c r="Y18" s="11"/>
       <c r="Z18" s="11"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>12</v>
@@ -2026,7 +2391,7 @@
         <v>10</v>
       </c>
       <c r="D19" s="7">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E19" s="13" t="s">
         <v>54</v>
@@ -2053,9 +2418,9 @@
       <c r="Y19" s="11"/>
       <c r="Z19" s="11"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>30</v>
@@ -2064,7 +2429,7 @@
         <v>10</v>
       </c>
       <c r="D20" s="7">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>56</v>
@@ -2091,9 +2456,9 @@
       <c r="Y20" s="11"/>
       <c r="Z20" s="11"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>13</v>
@@ -2102,7 +2467,7 @@
         <v>10</v>
       </c>
       <c r="D21" s="7">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
@@ -2127,9 +2492,9 @@
       <c r="Y21" s="11"/>
       <c r="Z21" s="11"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>15</v>
@@ -2138,7 +2503,7 @@
         <v>10</v>
       </c>
       <c r="D22" s="7">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
@@ -2163,7 +2528,7 @@
       <c r="Y22" s="11"/>
       <c r="Z22" s="11"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -2191,9 +2556,9 @@
       <c r="Y23" s="11"/>
       <c r="Z23" s="11"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>31</v>
@@ -2202,7 +2567,7 @@
         <v>32</v>
       </c>
       <c r="D24" s="7">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
@@ -2227,9 +2592,9 @@
       <c r="Y24" s="11"/>
       <c r="Z24" s="11"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>33</v>
@@ -2238,7 +2603,7 @@
         <v>32</v>
       </c>
       <c r="D25" s="7">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
@@ -2264,21 +2629,25 @@
       <c r="Z25" s="11"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="42.43"/>
+    <col min="2" max="2" width="42.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>68</v>
       </c>
@@ -2289,7 +2658,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -2297,14 +2666,14 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>46</v>
@@ -2313,12 +2682,12 @@
         <v>32</v>
       </c>
       <c r="D5" s="6">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>16</v>
@@ -2327,13 +2696,13 @@
         <v>10</v>
       </c>
       <c r="D6" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>40</v>
@@ -2342,17 +2711,17 @@
         <v>32</v>
       </c>
       <c r="D7" s="6">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>25</v>
@@ -2361,12 +2730,12 @@
         <v>10</v>
       </c>
       <c r="D11" s="6">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>31</v>
@@ -2375,12 +2744,12 @@
         <v>32</v>
       </c>
       <c r="D12" s="6">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>33</v>
@@ -2389,12 +2758,12 @@
         <v>32</v>
       </c>
       <c r="D13" s="6">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>36</v>
@@ -2403,12 +2772,12 @@
         <v>32</v>
       </c>
       <c r="D14" s="6">
-        <v>16.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>41</v>
@@ -2417,16 +2786,16 @@
         <v>32</v>
       </c>
       <c r="D15" s="15">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>72</v>
       </c>
@@ -2434,23 +2803,26 @@
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
     </row>
-    <row r="19">
-      <c r="A19" s="6">
-        <v>2.0</v>
-      </c>
-      <c r="B19" s="6" t="s">
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="18">
+        <v>2</v>
+      </c>
+      <c r="B19" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="6">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="20">
+      <c r="C19" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="18">
+        <v>8</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>38</v>
@@ -2459,12 +2831,12 @@
         <v>32</v>
       </c>
       <c r="D20" s="6">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>39</v>
@@ -2473,12 +2845,12 @@
         <v>32</v>
       </c>
       <c r="D21" s="6">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>26</v>
@@ -2487,33 +2859,37 @@
         <v>10</v>
       </c>
       <c r="D22" s="6">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C25" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D25" s="2">
-        <v>65.0</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13:D19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="39.29"/>
+    <col min="2" max="2" width="39.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="16" t="s">
         <v>73</v>
       </c>
@@ -2521,14 +2897,14 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>37</v>
@@ -2537,12 +2913,12 @@
         <v>32</v>
       </c>
       <c r="D6" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>44</v>
@@ -2551,37 +2927,40 @@
         <v>32</v>
       </c>
       <c r="D7" s="1">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="1">
-        <v>34.0</v>
-      </c>
-      <c r="B12" s="1" t="s">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="21">
+        <v>34</v>
+      </c>
+      <c r="B12" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="1">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="13">
+      <c r="D12" s="21">
+        <v>8</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>49</v>
@@ -2590,17 +2969,17 @@
         <v>32</v>
       </c>
       <c r="D13" s="1">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>34</v>
@@ -2609,12 +2988,12 @@
         <v>32</v>
       </c>
       <c r="D16" s="1">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>35</v>
@@ -2623,12 +3002,12 @@
         <v>32</v>
       </c>
       <c r="D17" s="1">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>2</v>
@@ -2637,12 +3016,12 @@
         <v>1</v>
       </c>
       <c r="D18" s="1">
-        <v>16.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>0</v>
@@ -2651,33 +3030,37 @@
         <v>1</v>
       </c>
       <c r="D19" s="1">
-        <v>16.0</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C22" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D22" s="2">
-        <v>61.0</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="40.0"/>
+    <col min="2" max="2" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="16" t="s">
         <v>77</v>
       </c>
@@ -2685,14 +3068,14 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>47</v>
@@ -2701,12 +3084,12 @@
         <v>32</v>
       </c>
       <c r="D5" s="1">
-        <v>16.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
@@ -2715,12 +3098,12 @@
         <v>1</v>
       </c>
       <c r="D6" s="3">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
@@ -2729,21 +3112,21 @@
         <v>1</v>
       </c>
       <c r="D7" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
@@ -2752,12 +3135,12 @@
         <v>1</v>
       </c>
       <c r="D11" s="1">
-        <v>16.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>4</v>
@@ -2766,18 +3149,19 @@
         <v>1</v>
       </c>
       <c r="D12" s="1">
-        <v>16.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C14" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D14" s="2">
-        <v>60.0</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>